<commit_message>
Update technical analysis files
</commit_message>
<xml_diff>
--- a/W-Advance_Technical_Analysis_QSE_STRONG_BUY.xlsx
+++ b/W-Advance_Technical_Analysis_QSE_STRONG_BUY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muhammadhafeez/Documents/GitHub/Python_PSX_Stock_Scanner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB87EAB-E22B-F140-8885-EDEB9FA78C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62EA08D-4519-4142-B742-88F6D8643B01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -726,11 +726,13 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -4047,7 +4049,7 @@
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>45381.108017859733</v>
+        <v>45381.473049682667</v>
       </c>
       <c r="B53" t="s">
         <v>74</v>
@@ -4103,7 +4105,7 @@
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
-        <v>45381.108017859733</v>
+        <v>45381.473049682667</v>
       </c>
       <c r="B54" t="s">
         <v>107</v>
@@ -4157,7 +4159,7 @@
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <v>45381.108017859733</v>
+        <v>45381.473049682667</v>
       </c>
       <c r="B55" t="s">
         <v>119</v>
@@ -4213,7 +4215,7 @@
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <v>45381.108017859733</v>
+        <v>45381.473049682667</v>
       </c>
       <c r="B56" t="s">
         <v>143</v>
@@ -4269,7 +4271,7 @@
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
-        <v>45381.108017859733</v>
+        <v>45381.473049682667</v>
       </c>
       <c r="B57" t="s">
         <v>167</v>
@@ -4325,7 +4327,7 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
-        <v>45381.108017859733</v>
+        <v>45381.473049682667</v>
       </c>
       <c r="B58" t="s">
         <v>179</v>
@@ -4381,7 +4383,7 @@
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
-        <v>45381.108017859733</v>
+        <v>45381.473049682667</v>
       </c>
       <c r="B59" t="s">
         <v>199</v>
@@ -4437,7 +4439,7 @@
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
-        <v>45381.108017859733</v>
+        <v>45381.473049682667</v>
       </c>
       <c r="B60" t="s">
         <v>223</v>
@@ -4511,25 +4513,12 @@
   <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="A5" sqref="A5:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="57.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="57" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
     <col min="18" max="18" width="50" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4756,7 +4745,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>45381.108017859733</v>
+        <v>45381.473049682667</v>
       </c>
       <c r="B5" t="s">
         <v>74</v>
@@ -4812,7 +4801,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>45381.108017859733</v>
+        <v>45381.473049682667</v>
       </c>
       <c r="B6" t="s">
         <v>119</v>
@@ -4868,7 +4857,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>45381.108017859733</v>
+        <v>45381.473049682667</v>
       </c>
       <c r="B7" t="s">
         <v>167</v>
@@ -4924,7 +4913,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>45381.108017859733</v>
+        <v>45381.473049682667</v>
       </c>
       <c r="B8" t="s">
         <v>179</v>
@@ -4980,7 +4969,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>45381.108017859733</v>
+        <v>45381.473049682667</v>
       </c>
       <c r="B9" t="s">
         <v>199</v>
@@ -5505,7 +5494,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>45381.108017859733</v>
+        <v>45381.473049682667</v>
       </c>
       <c r="B9" t="s">
         <v>119</v>
@@ -5561,7 +5550,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>45381.108017859733</v>
+        <v>45381.473049682667</v>
       </c>
       <c r="B10" t="s">
         <v>167</v>
@@ -5617,7 +5606,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>45381.108017859733</v>
+        <v>45381.473049682667</v>
       </c>
       <c r="B11" t="s">
         <v>179</v>
@@ -5673,7 +5662,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>45381.108017859733</v>
+        <v>45381.473049682667</v>
       </c>
       <c r="B12" t="s">
         <v>199</v>
@@ -7731,7 +7720,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>45381.108017859733</v>
+        <v>45381.473049682667</v>
       </c>
       <c r="B13" t="s">
         <v>74</v>
@@ -7787,7 +7776,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>45381.108017859733</v>
+        <v>45381.473049682667</v>
       </c>
       <c r="B14" t="s">
         <v>119</v>
@@ -7843,7 +7832,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>45381.108017859733</v>
+        <v>45381.473049682667</v>
       </c>
       <c r="B15" t="s">
         <v>167</v>
@@ -7899,7 +7888,7 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>45381.108017859733</v>
+        <v>45381.473049682667</v>
       </c>
       <c r="B16" t="s">
         <v>179</v>
@@ -7955,7 +7944,7 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>45381.108017859733</v>
+        <v>45381.473049682667</v>
       </c>
       <c r="B17" t="s">
         <v>199</v>
@@ -8011,7 +8000,7 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>45381.108017859733</v>
+        <v>45381.473049682667</v>
       </c>
       <c r="B18" t="s">
         <v>223</v>

</xml_diff>